<commit_message>
+updated exceptions and status
</commit_message>
<xml_diff>
--- a/Data/Input/Question1.xlsx
+++ b/Data/Input/Question1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Day11_Assignment2\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDE78AA-57FB-4FB0-A232-5E80B7754DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AE769E-39EE-4AD2-BD93-97DA1A786793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="2250" yWindow="2250" windowWidth="18000" windowHeight="9360" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <x:sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <x:sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <x:sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <x:sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="124519"/>
@@ -1558,7 +1558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0100-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -1577,18 +1577,739 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:F36"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:sheetData/>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
+      <x:c r="A2" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="A8" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="A9" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="A10" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="A12" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="A13" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="A14" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="A15" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="A16" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="A17" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="A18" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="A19" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="A20" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="A21" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="A22" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="A23" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="A24" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6">
+      <x:c r="A25" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="A26" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="A27" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="A28" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="A29" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="A30" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="A31" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="A32" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="A33" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="A34" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="F34" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="A35" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="A36" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="F36" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>

</xml_diff>